<commit_message>
Windows handles and frame
</commit_message>
<xml_diff>
--- a/Docs_files/Excels/ExcelWrite.xlsx
+++ b/Docs_files/Excels/ExcelWrite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>one</t>
   </si>
@@ -114,6 +114,216 @@
   </si>
   <si>
     <t>twenty-eight</t>
+  </si>
+  <si>
+    <t>thirty-one</t>
+  </si>
+  <si>
+    <t>thirty-two</t>
+  </si>
+  <si>
+    <t>thirty-three</t>
+  </si>
+  <si>
+    <t>thirty-four</t>
+  </si>
+  <si>
+    <t>thirty-five</t>
+  </si>
+  <si>
+    <t>thirty-six</t>
+  </si>
+  <si>
+    <t>thirty-seven</t>
+  </si>
+  <si>
+    <t>thirty-eight</t>
+  </si>
+  <si>
+    <t>thirty-nine</t>
+  </si>
+  <si>
+    <t>forty</t>
+  </si>
+  <si>
+    <t>forty-one</t>
+  </si>
+  <si>
+    <t>forty-two</t>
+  </si>
+  <si>
+    <t>forty-three</t>
+  </si>
+  <si>
+    <t>forty-four</t>
+  </si>
+  <si>
+    <t>forty-five</t>
+  </si>
+  <si>
+    <t>forty-six</t>
+  </si>
+  <si>
+    <t>forty-seven</t>
+  </si>
+  <si>
+    <t>forty-eight</t>
+  </si>
+  <si>
+    <t>forty-nine</t>
+  </si>
+  <si>
+    <t>fifty-two</t>
+  </si>
+  <si>
+    <t>fifty-three</t>
+  </si>
+  <si>
+    <t>fifty-four</t>
+  </si>
+  <si>
+    <t>fifty-five</t>
+  </si>
+  <si>
+    <t>fifty-six</t>
+  </si>
+  <si>
+    <t>fifty-seven</t>
+  </si>
+  <si>
+    <t>fifty-eight</t>
+  </si>
+  <si>
+    <t>fifty-nine</t>
+  </si>
+  <si>
+    <t>fifty-one</t>
+  </si>
+  <si>
+    <t>sixty-two</t>
+  </si>
+  <si>
+    <t>sixty-three</t>
+  </si>
+  <si>
+    <t>sixty-four</t>
+  </si>
+  <si>
+    <t>sixty-five</t>
+  </si>
+  <si>
+    <t>sixty-six</t>
+  </si>
+  <si>
+    <t>sixty-seven</t>
+  </si>
+  <si>
+    <t>sixty-eight</t>
+  </si>
+  <si>
+    <t>sixty-nine</t>
+  </si>
+  <si>
+    <t>sixty-one</t>
+  </si>
+  <si>
+    <t>seventy-one</t>
+  </si>
+  <si>
+    <t>seventy-two</t>
+  </si>
+  <si>
+    <t>seventy-three</t>
+  </si>
+  <si>
+    <t>seventy-four</t>
+  </si>
+  <si>
+    <t>seventy-five</t>
+  </si>
+  <si>
+    <t>seventy-six</t>
+  </si>
+  <si>
+    <t>seventy-seven</t>
+  </si>
+  <si>
+    <t>seventy-eight</t>
+  </si>
+  <si>
+    <t>seventy-nine</t>
+  </si>
+  <si>
+    <t>fifty</t>
+  </si>
+  <si>
+    <t>sixty</t>
+  </si>
+  <si>
+    <t>seventy</t>
+  </si>
+  <si>
+    <t>eighty</t>
+  </si>
+  <si>
+    <t>eighty-two</t>
+  </si>
+  <si>
+    <t>eighty-three</t>
+  </si>
+  <si>
+    <t>eighty-four</t>
+  </si>
+  <si>
+    <t>eighty-five</t>
+  </si>
+  <si>
+    <t>eighty-six</t>
+  </si>
+  <si>
+    <t>eighty-seven</t>
+  </si>
+  <si>
+    <t>eighty-eight</t>
+  </si>
+  <si>
+    <t>eighty-nine</t>
+  </si>
+  <si>
+    <t>eighty-one</t>
+  </si>
+  <si>
+    <t>ninety</t>
+  </si>
+  <si>
+    <t>ninety-one</t>
+  </si>
+  <si>
+    <t>ninety-two</t>
+  </si>
+  <si>
+    <t>ninety-three</t>
+  </si>
+  <si>
+    <t>ninety-four</t>
+  </si>
+  <si>
+    <t>ninety-five</t>
+  </si>
+  <si>
+    <t>ninety-six</t>
+  </si>
+  <si>
+    <t>ninety-seven</t>
+  </si>
+  <si>
+    <t>ninety-eight</t>
+  </si>
+  <si>
+    <t>ninety-nine</t>
+  </si>
+  <si>
+    <t>hundred</t>
   </si>
 </sst>
 </file>
@@ -149,8 +359,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,274 +644,375 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="1">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="1">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" s="1">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" s="1">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H1" s="1">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="I1" s="1">
         <v>9</v>
+      </c>
+      <c r="J1" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>6</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
-      </c>
-      <c r="I4">
-        <v>6</v>
-      </c>
-      <c r="J4">
-        <v>6</v>
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>7</v>
-      </c>
-      <c r="G5">
-        <v>7</v>
-      </c>
-      <c r="H5">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <v>7</v>
-      </c>
-      <c r="J5">
-        <v>7</v>
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <v>8</v>
-      </c>
-      <c r="F6">
-        <v>8</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <v>8</v>
-      </c>
-      <c r="J6">
-        <v>8</v>
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>9</v>
-      </c>
-      <c r="E7">
-        <v>9</v>
-      </c>
-      <c r="F7">
-        <v>9</v>
-      </c>
-      <c r="G7">
-        <v>9</v>
-      </c>
-      <c r="H7">
-        <v>9</v>
-      </c>
-      <c r="I7">
-        <v>9</v>
-      </c>
-      <c r="J7">
-        <v>9</v>
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
-      <c r="H8">
-        <v>10</v>
-      </c>
-      <c r="I8">
-        <v>10</v>
-      </c>
-      <c r="J8">
-        <v>10</v>
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" t="s">
+        <v>87</v>
+      </c>
+      <c r="J10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H11" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>